<commit_message>
BATS delete functionality added
</commit_message>
<xml_diff>
--- a/resources/Chart Setting.xlsx
+++ b/resources/Chart Setting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aamna\Documents\AbdulazizNahas\AbdulazizNahas\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F890173C-E987-4A5F-9CF3-0F766A6AC913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0146107-74FE-4487-A75A-39531A9BE3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,15 +559,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="33.9453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="17.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.55000000000000004">

</xml_diff>